<commit_message>
se arregla un erro de clase en agregarprodcuto.js
</commit_message>
<xml_diff>
--- a/documentacion_del_proyecto/Matriz de seguimiento.xlsx
+++ b/documentacion_del_proyecto/Matriz de seguimiento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsung\OneDrive\Escritorio\hola\R_Universisdad_Segunda_Mano\documentacion_del_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00645DB-A480-4348-99E5-4BA8DFDBC3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -98,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,22 +601,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -636,7 +628,7 @@
       <c r="E1" s="12"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="6" t="s">
@@ -653,67 +645,67 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -725,7 +717,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -737,7 +729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -749,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -761,7 +753,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
@@ -773,7 +765,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -785,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -797,7 +789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Arregla faltas de ortografía
</commit_message>
<xml_diff>
--- a/documentacion_del_proyecto/Matriz de seguimiento.xlsx
+++ b/documentacion_del_proyecto/Matriz de seguimiento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsung\OneDrive\Escritorio\hola\R_Universisdad_Segunda_Mano\documentacion_del_proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cf206\OneDrive\Desktop\scuele\R_Universisdad_Segunda_Mano\documentacion_del_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00645DB-A480-4348-99E5-4BA8DFDBC3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1382588A-3CFE-4FD9-AEDC-8BDB91414A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -42,49 +42,49 @@
     <t>Poco terminado</t>
   </si>
   <si>
-    <t>Sin Empesar</t>
-  </si>
-  <si>
-    <t>Pagina Inicial(Index)</t>
-  </si>
-  <si>
-    <t>inicio de secion</t>
-  </si>
-  <si>
-    <t>registro de usuario</t>
-  </si>
-  <si>
-    <t>carro de coompras</t>
-  </si>
-  <si>
-    <t>vender</t>
-  </si>
-  <si>
-    <t>nosotros</t>
-  </si>
-  <si>
-    <t>forma de pago</t>
-  </si>
-  <si>
-    <t>pagina de los productos</t>
-  </si>
-  <si>
-    <t>perfil de usuario</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
     <t>Favoritos</t>
   </si>
   <si>
-    <t>seccion de electronica</t>
-  </si>
-  <si>
-    <t>seccion de anime</t>
-  </si>
-  <si>
-    <t>Pagina inicial usuario</t>
+    <t>Inicio de sesión</t>
+  </si>
+  <si>
+    <t>Página inicial usuario</t>
+  </si>
+  <si>
+    <t>Registro de usuario</t>
+  </si>
+  <si>
+    <t>Forma de pago</t>
+  </si>
+  <si>
+    <t>Vender</t>
+  </si>
+  <si>
+    <t>Nosotros</t>
+  </si>
+  <si>
+    <t>Perfil de usuario</t>
+  </si>
+  <si>
+    <t>Seccion de anime</t>
+  </si>
+  <si>
+    <t>Carro de compras</t>
+  </si>
+  <si>
+    <t>Página de los productos</t>
+  </si>
+  <si>
+    <t>Seccion de electrónica</t>
+  </si>
+  <si>
+    <t>Sin empezar</t>
+  </si>
+  <si>
+    <t>Página Inicial (Index)</t>
   </si>
 </sst>
 </file>
@@ -306,9 +306,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -346,7 +346,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -452,7 +452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -594,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -605,7 +605,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,17 +641,17 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -659,11 +659,11 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -675,7 +675,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -683,11 +683,11 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -695,11 +695,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -707,86 +707,86 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -798,7 +798,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -820,5 +820,6 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>